<commit_message>
Add new test cases and datasets for Naive Bayes implementation; refactor existing CSV files and balance dataset
</commit_message>
<xml_diff>
--- a/Navie Bayesian/test.xlsx
+++ b/Navie Bayesian/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgh99\Desktop\python\ML\24-2-ML\Navie Bayesian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E524F366-613F-4875-9A4C-04C1CD36B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271A1029-9806-48D9-8A31-85229D9AE92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="3465" windowWidth="23670" windowHeight="15345" xr2:uid="{4A677B36-5DA1-4683-BF1A-F5B76569DB3A}"/>
+    <workbookView xWindow="40215" yWindow="4080" windowWidth="23670" windowHeight="15345" xr2:uid="{4A677B36-5DA1-4683-BF1A-F5B76569DB3A}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1499,10 +1499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1">
@@ -1512,9 +1512,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1544,10 +1541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1565,26 +1559,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1961,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4429D685-3C2B-441F-B4F9-3BA95EB4D251}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1978,7 +1999,7 @@
     <col min="16" max="16" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2012,7 +2033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2029,7 +2050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +2067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2063,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +2101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2114,7 +2135,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2131,7 +2152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2148,7 +2169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2167,8 +2188,11 @@
       <c r="I11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="O11" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2187,11 +2211,9 @@
       <c r="I12" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2207,9 +2229,11 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="13"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="O13" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2228,11 +2252,11 @@
       <c r="I14" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="O14" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2251,19 +2275,19 @@
       <c r="I15" t="s">
         <v>76</v>
       </c>
-      <c r="Q15" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="O15" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="I16" t="s">
         <v>79</v>
       </c>
-      <c r="Q16" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="O16" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2273,12 +2297,9 @@
       <c r="I17" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="17.25" thickBot="1"/>
-    <row r="19" spans="1:17" ht="17.25" thickBot="1">
+    </row>
+    <row r="18" spans="1:16" ht="17.25" thickBot="1"/>
+    <row r="19" spans="1:16" ht="17.25" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -2297,32 +2318,32 @@
       <c r="G19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="32" t="s">
+      <c r="L19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="M19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="32" t="s">
+      <c r="N19" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="32" t="s">
+      <c r="O19" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="P19" s="33" t="s">
+      <c r="P19" s="41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -2341,32 +2362,32 @@
       <c r="G20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="28">
         <v>3</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="28">
         <v>9</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="28">
         <v>3</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="28">
         <v>2</v>
       </c>
-      <c r="P20" s="28" t="s">
+      <c r="P20" s="30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="17.25" thickBot="1">
+    <row r="21" spans="1:16" ht="17.25" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2385,32 +2406,32 @@
       <c r="G21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="32">
         <v>3</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="32">
         <v>9</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="32">
         <v>4</v>
       </c>
-      <c r="N21" s="21" t="s">
+      <c r="N21" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="32">
         <v>0</v>
       </c>
-      <c r="P21" s="29" t="s">
+      <c r="P21" s="34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="17.25" thickBot="1">
+    <row r="22" spans="1:16" ht="17.25" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -2420,42 +2441,42 @@
       <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="36">
         <v>3</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="36">
         <v>9</v>
       </c>
-      <c r="L22" s="26" t="s">
+      <c r="L22" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="36">
         <v>2</v>
       </c>
-      <c r="N22" s="25" t="s">
+      <c r="N22" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="O22" s="25">
+      <c r="O22" s="36">
         <v>3</v>
       </c>
-      <c r="P22" s="30" t="s">
+      <c r="P22" s="38" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="17.25" thickBot="1">
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-    </row>
-    <row r="24" spans="1:17">
+    <row r="23" spans="1:16" ht="17.25" thickBot="1">
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -2474,32 +2495,32 @@
       <c r="G24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="16">
         <v>3</v>
       </c>
-      <c r="K24" s="17">
+      <c r="K24" s="16">
         <v>9</v>
       </c>
-      <c r="L24" s="34" t="s">
+      <c r="L24" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="M24" s="17">
+      <c r="M24" s="16">
         <v>2</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N24" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="O24" s="17">
+      <c r="O24" s="16">
         <v>2</v>
       </c>
-      <c r="P24" s="19" t="s">
+      <c r="P24" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:16">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -2518,32 +2539,32 @@
       <c r="G25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="14">
         <v>3</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="14">
         <v>9</v>
       </c>
-      <c r="L25" s="22" t="s">
+      <c r="L25" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="14">
         <v>4</v>
       </c>
-      <c r="N25" s="22" t="s">
+      <c r="N25" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="O25" s="21">
+      <c r="O25" s="14">
         <v>2</v>
       </c>
-      <c r="P25" s="23" t="s">
+      <c r="P25" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="17.25" thickBot="1">
+    <row r="26" spans="1:16" ht="17.25" thickBot="1">
       <c r="A26" s="4" t="s">
         <v>10</v>
       </c>
@@ -2562,32 +2583,32 @@
       <c r="G26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I26" s="24" t="s">
+      <c r="I26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="23">
         <v>3</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="23">
         <v>9</v>
       </c>
-      <c r="L26" s="26" t="s">
+      <c r="L26" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="23">
         <v>3</v>
       </c>
-      <c r="N26" s="26" t="s">
+      <c r="N26" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="O26" s="25">
+      <c r="O26" s="23">
         <v>1</v>
       </c>
-      <c r="P26" s="27" t="s">
+      <c r="P26" s="25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="17.25" thickBot="1">
+    <row r="27" spans="1:16" ht="17.25" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -2597,126 +2618,126 @@
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="I28" s="16" t="s">
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="I28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="16">
         <v>2</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="16">
         <v>9</v>
       </c>
-      <c r="L28" s="18" t="s">
+      <c r="L28" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M28" s="16">
         <v>3</v>
       </c>
-      <c r="N28" s="18" t="s">
+      <c r="N28" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O28" s="17">
+      <c r="O28" s="16">
         <v>4</v>
       </c>
-      <c r="P28" s="19" t="s">
+      <c r="P28" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="17.25" thickBot="1">
-      <c r="I29" s="24" t="s">
+    <row r="29" spans="1:16" ht="17.25" thickBot="1">
+      <c r="I29" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="23">
         <v>2</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="23">
         <v>9</v>
       </c>
-      <c r="L29" s="26" t="s">
+      <c r="L29" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="23">
         <v>6</v>
       </c>
-      <c r="N29" s="26" t="s">
+      <c r="N29" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="O29" s="25">
+      <c r="O29" s="23">
         <v>1</v>
       </c>
-      <c r="P29" s="27" t="s">
+      <c r="P29" s="25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="17.25" thickBot="1">
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="I31" s="16" t="b">
+    <row r="30" spans="1:16" ht="17.25" thickBot="1">
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="I31" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="16">
         <v>2</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <v>9</v>
       </c>
-      <c r="L31" s="18" t="s">
+      <c r="L31" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="M31" s="17">
+      <c r="M31" s="16">
         <v>3</v>
       </c>
-      <c r="N31" s="18" t="s">
+      <c r="N31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O31" s="17">
+      <c r="O31" s="16">
         <v>3</v>
       </c>
-      <c r="P31" s="19" t="s">
+      <c r="P31" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="17.25" thickBot="1">
-      <c r="I32" s="24" t="b">
+    <row r="32" spans="1:16" ht="17.25" thickBot="1">
+      <c r="I32" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="23">
         <v>2</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="23">
         <v>9</v>
       </c>
-      <c r="L32" s="26" t="s">
+      <c r="L32" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="M32" s="25">
+      <c r="M32" s="23">
         <v>6</v>
       </c>
-      <c r="N32" s="26" t="s">
+      <c r="N32" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="O32" s="25">
+      <c r="O32" s="23">
         <v>2</v>
       </c>
-      <c r="P32" s="27" t="s">
+      <c r="P32" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2732,7 +2753,7 @@
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="G35" t="s">
@@ -2746,7 +2767,7 @@
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="G36" t="s">
@@ -2823,5 +2844,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>